<commit_message>
final version for handing in my report
</commit_message>
<xml_diff>
--- a/python sim/animation_eval.xlsx
+++ b/python sim/animation_eval.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Desktop\CP2\workspace\python sim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADA4064-5B87-4579-97C7-5C33D76727A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15FFB711-C616-4CE5-BEE7-0796876A25CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="885" yWindow="1620" windowWidth="21570" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="10">
   <si>
     <t>R</t>
   </si>
@@ -43,13 +56,13 @@
     <t>PREDICTION</t>
   </si>
   <si>
-    <t>not clear</t>
-  </si>
-  <si>
     <t>upload</t>
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>0.524….</t>
   </si>
 </sst>
 </file>
@@ -426,8 +439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,11 +467,13 @@
         <v>6</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
       <c r="B2">
         <v>3.47</v>
       </c>
@@ -469,14 +484,16 @@
         <v>0.52359877559829882</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
       <c r="B3">
         <v>4</v>
       </c>
@@ -490,11 +507,13 @@
         <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
       <c r="B4">
         <v>4</v>
       </c>
@@ -508,11 +527,13 @@
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
       <c r="B5">
         <v>5</v>
       </c>
@@ -526,11 +547,13 @@
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
       <c r="B6">
         <v>5</v>
       </c>
@@ -544,11 +567,13 @@
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
       <c r="B7">
         <v>5</v>
       </c>
@@ -562,11 +587,13 @@
         <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
       <c r="B8">
         <v>5</v>
       </c>
@@ -580,11 +607,13 @@
         <v>5</v>
       </c>
       <c r="G8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
       <c r="B9">
         <v>5.5</v>
       </c>
@@ -598,11 +627,13 @@
         <v>4</v>
       </c>
       <c r="G9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
       <c r="B10">
         <v>5.5</v>
       </c>
@@ -613,14 +644,16 @@
         <v>0.48869219055841229</v>
       </c>
       <c r="E10" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
       <c r="B11">
         <v>6</v>
       </c>
@@ -631,14 +664,16 @@
         <v>0.26179938779914941</v>
       </c>
       <c r="E11" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
       <c r="B12">
         <v>6</v>
       </c>
@@ -652,11 +687,13 @@
         <v>4</v>
       </c>
       <c r="G12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
       <c r="B13">
         <v>7</v>
       </c>
@@ -670,11 +707,13 @@
         <v>5</v>
       </c>
       <c r="G13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
       <c r="B14">
         <v>7</v>
       </c>
@@ -688,11 +727,13 @@
         <v>4</v>
       </c>
       <c r="G14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
       <c r="B15">
         <v>8</v>
       </c>
@@ -702,9 +743,17 @@
       <c r="D15">
         <v>0.26179938779914941</v>
       </c>
+      <c r="E15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
       <c r="B16">
         <v>8</v>
       </c>
@@ -714,45 +763,101 @@
       <c r="D16">
         <v>0.19198621771937621</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
       <c r="B17">
         <v>9</v>
       </c>
       <c r="C17">
         <v>6</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
+      <c r="D17">
+        <f>RADIANS(C17)</f>
+        <v>0.10471975511965978</v>
+      </c>
+      <c r="E17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
       <c r="B18">
         <v>9</v>
       </c>
       <c r="C18">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
+      <c r="D18">
+        <f>RADIANS(C18)</f>
+        <v>0.38397243543875248</v>
+      </c>
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
       <c r="B19">
         <v>10</v>
       </c>
       <c r="C19">
         <v>8</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
+      <c r="D19">
+        <f>RADIANS(C19)</f>
+        <v>0.13962634015954636</v>
+      </c>
+      <c r="E19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
       <c r="B20">
         <v>10</v>
       </c>
       <c r="C20">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
+      <c r="D20">
+        <f>RADIANS(C20)</f>
+        <v>0.22689280275926285</v>
+      </c>
+      <c r="E20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
       <c r="B21">
         <v>12</v>
       </c>
@@ -762,9 +867,17 @@
       <c r="D21">
         <v>0.10471975511965979</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
+      <c r="E21" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
       <c r="B22">
         <v>12</v>
       </c>
@@ -774,18 +887,37 @@
       <c r="D22">
         <v>0.19198621771937621</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
+      <c r="E22" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
       <c r="B23">
         <v>12</v>
       </c>
       <c r="C23">
         <v>30</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" t="s">
+        <v>5</v>
+      </c>
+      <c r="G23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
       <c r="B24">
         <v>14</v>
       </c>
@@ -794,6 +926,12 @@
       </c>
       <c r="D24">
         <v>0.1308996938995747</v>
+      </c>
+      <c r="E24" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>